<commit_message>
Integration quasi complete de la creation de tableau sur les commandes (manque plus que devoir), creation de lentrée 'correction' dans le tableau de reception, amelioration de correction, suppression de l'envoi différé
</commit_message>
<xml_diff>
--- a/Hmw_tables/math .xlsx
+++ b/Hmw_tables/math .xlsx
@@ -14,12 +14,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="9">
   <si>
     <t>activité 1</t>
-  </si>
-  <si>
-    <t>activité 2</t>
   </si>
   <si>
     <t>activité 23</t>
@@ -31,7 +28,7 @@
     <t>sloth</t>
   </si>
   <si>
-    <t>le 05/16 à 11h53</t>
+    <t>Corrigé</t>
   </si>
   <si>
     <t>skido</t>
@@ -94,7 +91,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA9D08E"/>
+        <fgColor rgb="FFFF6347"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -138,7 +135,7 @@
       <alignment horizontal="justify"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -443,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -453,9 +450,9 @@
     <col min="2" max="702" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -463,538 +460,346 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="3" t="s">
+      <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
       <c r="A24" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
       <c r="A26" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correctif d'un oubli (prise en compte du bon nom et optimisation du code
</commit_message>
<xml_diff>
--- a/Hmw_tables/math .xlsx
+++ b/Hmw_tables/math .xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="47">
   <si>
     <t>activité 23</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Élèves</t>
   </si>
   <si>
-    <t>sloth</t>
+    <t>Sloth</t>
   </si>
   <si>
     <t>Non rendu</t>
@@ -43,121 +43,118 @@
     <t>Corrigé</t>
   </si>
   <si>
-    <t>le 05/16 à 11h53</t>
-  </si>
-  <si>
-    <t>skido</t>
-  </si>
-  <si>
-    <t>alexis</t>
-  </si>
-  <si>
-    <t>amelie</t>
-  </si>
-  <si>
-    <t>baptiste</t>
-  </si>
-  <si>
-    <t>axelle</t>
-  </si>
-  <si>
-    <t>bastian</t>
-  </si>
-  <si>
-    <t>camille</t>
-  </si>
-  <si>
-    <t>charlie</t>
-  </si>
-  <si>
-    <t>emeline</t>
-  </si>
-  <si>
-    <t>emile</t>
-  </si>
-  <si>
-    <t>enzo</t>
-  </si>
-  <si>
-    <t>florian</t>
-  </si>
-  <si>
-    <t>gregoire</t>
-  </si>
-  <si>
-    <t>hugo</t>
-  </si>
-  <si>
-    <t>jason</t>
-  </si>
-  <si>
-    <t>jean</t>
-  </si>
-  <si>
-    <t>juan</t>
-  </si>
-  <si>
-    <t>louis</t>
-  </si>
-  <si>
-    <t>lea</t>
-  </si>
-  <si>
-    <t>leo</t>
-  </si>
-  <si>
-    <t>manon</t>
-  </si>
-  <si>
-    <t>margauxl</t>
-  </si>
-  <si>
-    <t>margauxq</t>
-  </si>
-  <si>
-    <t>marie</t>
-  </si>
-  <si>
-    <t>mateo</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>maxence</t>
-  </si>
-  <si>
-    <t>mael</t>
-  </si>
-  <si>
-    <t>pierre</t>
-  </si>
-  <si>
-    <t>romain</t>
-  </si>
-  <si>
-    <t>sarah</t>
-  </si>
-  <si>
-    <t>theog</t>
-  </si>
-  <si>
-    <t>theob</t>
-  </si>
-  <si>
-    <t>thibaut</t>
-  </si>
-  <si>
-    <t>vivien</t>
-  </si>
-  <si>
-    <t>ambre</t>
-  </si>
-  <si>
-    <t>margauxo</t>
-  </si>
-  <si>
-    <t>mona</t>
+    <t>Skido</t>
+  </si>
+  <si>
+    <t>Alexis</t>
+  </si>
+  <si>
+    <t>Amelie</t>
+  </si>
+  <si>
+    <t>Baptiste</t>
+  </si>
+  <si>
+    <t>Axelle</t>
+  </si>
+  <si>
+    <t>Bastian</t>
+  </si>
+  <si>
+    <t>Camille</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Emeline</t>
+  </si>
+  <si>
+    <t>Emile</t>
+  </si>
+  <si>
+    <t>Enzo</t>
+  </si>
+  <si>
+    <t>Florian</t>
+  </si>
+  <si>
+    <t>Gregoire</t>
+  </si>
+  <si>
+    <t>Hugo</t>
+  </si>
+  <si>
+    <t>Jason</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Lea</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Manon</t>
+  </si>
+  <si>
+    <t>Margauxl</t>
+  </si>
+  <si>
+    <t>Margauxq</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Mateo</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Maxence</t>
+  </si>
+  <si>
+    <t>Mael</t>
+  </si>
+  <si>
+    <t>Pierre</t>
+  </si>
+  <si>
+    <t>Romain</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Theog</t>
+  </si>
+  <si>
+    <t>Theob</t>
+  </si>
+  <si>
+    <t>Thibaut</t>
+  </si>
+  <si>
+    <t>Vivien</t>
+  </si>
+  <si>
+    <t>Ambre</t>
+  </si>
+  <si>
+    <t>Margauxo</t>
+  </si>
+  <si>
+    <t>Mona</t>
   </si>
 </sst>
 </file>
@@ -181,7 +178,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,12 +215,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA9D08E"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -252,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -267,9 +258,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -612,13 +600,13 @@
       <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>9</v>
+      <c r="F2" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
@@ -638,7 +626,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
@@ -652,13 +640,13 @@
       <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>9</v>
+      <c r="F4" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
@@ -672,13 +660,13 @@
       <c r="E5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>9</v>
+      <c r="F5" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
@@ -692,13 +680,13 @@
       <c r="E6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>9</v>
+      <c r="F6" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
@@ -712,13 +700,13 @@
       <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>9</v>
+      <c r="F7" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
@@ -732,13 +720,13 @@
       <c r="E8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>9</v>
+      <c r="F8" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
@@ -752,13 +740,13 @@
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>9</v>
+      <c r="F9" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
@@ -772,13 +760,13 @@
       <c r="E10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>9</v>
+      <c r="F10" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
@@ -792,13 +780,13 @@
       <c r="E11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>9</v>
+      <c r="F11" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
@@ -812,13 +800,13 @@
       <c r="E12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>9</v>
+      <c r="F12" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>7</v>
@@ -832,13 +820,13 @@
       <c r="E13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>9</v>
+      <c r="F13" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
@@ -852,13 +840,13 @@
       <c r="E14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>9</v>
+      <c r="F14" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
@@ -872,13 +860,13 @@
       <c r="E15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>9</v>
+      <c r="F15" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
@@ -892,13 +880,13 @@
       <c r="E16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>9</v>
+      <c r="F16" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
@@ -912,13 +900,13 @@
       <c r="E17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>9</v>
+      <c r="F17" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>7</v>
@@ -932,13 +920,13 @@
       <c r="E18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>9</v>
+      <c r="F18" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>7</v>
@@ -952,13 +940,13 @@
       <c r="E19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>9</v>
+      <c r="F19" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
@@ -972,13 +960,13 @@
       <c r="E20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>9</v>
+      <c r="F20" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>7</v>
@@ -992,13 +980,13 @@
       <c r="E21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>9</v>
+      <c r="F21" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>7</v>
@@ -1012,13 +1000,13 @@
       <c r="E22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>9</v>
+      <c r="F22" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>7</v>
@@ -1032,13 +1020,13 @@
       <c r="E23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>9</v>
+      <c r="F23" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>7</v>
@@ -1052,13 +1040,13 @@
       <c r="E24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>9</v>
+      <c r="F24" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>7</v>
@@ -1072,13 +1060,13 @@
       <c r="E25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="6" t="s">
-        <v>9</v>
+      <c r="F25" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>7</v>
@@ -1092,13 +1080,13 @@
       <c r="E26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F26" s="6" t="s">
-        <v>9</v>
+      <c r="F26" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>7</v>
@@ -1112,13 +1100,13 @@
       <c r="E27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>9</v>
+      <c r="F27" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>7</v>
@@ -1132,13 +1120,13 @@
       <c r="E28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="6" t="s">
-        <v>9</v>
+      <c r="F28" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>7</v>
@@ -1152,13 +1140,13 @@
       <c r="E29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F29" s="6" t="s">
-        <v>9</v>
+      <c r="F29" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>7</v>
@@ -1172,13 +1160,13 @@
       <c r="E30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>9</v>
+      <c r="F30" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>7</v>
@@ -1192,13 +1180,13 @@
       <c r="E31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>9</v>
+      <c r="F31" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>7</v>
@@ -1212,13 +1200,13 @@
       <c r="E32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>9</v>
+      <c r="F32" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>7</v>
@@ -1232,13 +1220,13 @@
       <c r="E33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>9</v>
+      <c r="F33" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>7</v>
@@ -1252,13 +1240,13 @@
       <c r="E34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="6" t="s">
-        <v>9</v>
+      <c r="F34" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>7</v>
@@ -1272,13 +1260,13 @@
       <c r="E35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>9</v>
+      <c r="F35" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>7</v>
@@ -1292,13 +1280,13 @@
       <c r="E36" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>9</v>
+      <c r="F36" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>7</v>
@@ -1312,13 +1300,13 @@
       <c r="E37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="6" t="s">
-        <v>9</v>
+      <c r="F37" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>7</v>
@@ -1332,13 +1320,13 @@
       <c r="E38" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F38" s="6" t="s">
-        <v>9</v>
+      <c r="F38" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>7</v>
@@ -1352,13 +1340,13 @@
       <c r="E39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F39" s="6" t="s">
-        <v>9</v>
+      <c r="F39" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>7</v>
@@ -1372,8 +1360,8 @@
       <c r="E40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F40" s="6" t="s">
-        <v>9</v>
+      <c r="F40" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>